<commit_message>
Commiting Create Class Functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/programBook.xlsx
+++ b/src/test/resources/testData/programBook.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ani\selenium_projects\Team2_AssuredNinjas\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\subha\git\Team2_AssuredNinjas_L\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A947D86E-FB81-4C0A-93C6-91DF8C290273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF41031-BCEE-4D19-B9C6-9C6508ACD4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2D91261-AFF6-46E2-95E7-14861063D73C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{A2D91261-AFF6-46E2-95E7-14861063D73C}"/>
   </bookViews>
   <sheets>
     <sheet name="programModule" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="classModule" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Scenarios</t>
   </si>
@@ -117,19 +117,82 @@
   </si>
   <si>
     <t>nonstaticcoding</t>
+  </si>
+  <si>
+    <t>batchId</t>
+  </si>
+  <si>
+    <t>classNo</t>
+  </si>
+  <si>
+    <t>classDate</t>
+  </si>
+  <si>
+    <t>classTopic</t>
+  </si>
+  <si>
+    <t>classStatus</t>
+  </si>
+  <si>
+    <t>classStaffId</t>
+  </si>
+  <si>
+    <t>classDescription</t>
+  </si>
+  <si>
+    <t>classComments</t>
+  </si>
+  <si>
+    <t>classNotes</t>
+  </si>
+  <si>
+    <t>classRecordingPath</t>
+  </si>
+  <si>
+    <t>classScheduledDates</t>
+  </si>
+  <si>
+    <t>2025-04-25T15:11:08.750Z</t>
+  </si>
+  <si>
+    <t>assuredNinjasfourone</t>
+  </si>
+  <si>
+    <t>U3718</t>
+  </si>
+  <si>
+    <t>Subha classDescription</t>
+  </si>
+  <si>
+    <t>classcreate comments</t>
+  </si>
+  <si>
+    <t>Subha Notes</t>
+  </si>
+  <si>
+    <t>D://Downloads</t>
+  </si>
+  <si>
+    <t>2025-05-25T15:11:08.750Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,10 +203,36 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -152,8 +241,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,22 +564,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0079617B-323A-45A1-95E5-CB9189128ADF}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="29.109375" customWidth="1"/>
+    <col min="1" max="1" width="29.36328125" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+    <col min="5" max="5" width="29.08984375" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +602,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -531,7 +625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -554,7 +648,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -568,7 +662,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -579,7 +673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -600,12 +694,106 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0156936-DD37-4927-B652-D0EEE57BE1A4}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.08984375" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="21.90625" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" customWidth="1"/>
+    <col min="5" max="5" width="20.90625" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" customWidth="1"/>
+    <col min="8" max="8" width="33.36328125" customWidth="1"/>
+    <col min="9" max="9" width="21.90625" customWidth="1"/>
+    <col min="10" max="10" width="20.7265625" customWidth="1"/>
+    <col min="11" max="11" width="21.08984375" customWidth="1"/>
+    <col min="12" max="12" width="23.36328125" customWidth="1"/>
+    <col min="13" max="13" width="27.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>12407</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -616,7 +804,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>